<commit_message>
add ejscreen data processing function
</commit_message>
<xml_diff>
--- a/data/ejscreen/ejscreen_meta.xlsx
+++ b/data/ejscreen/ejscreen_meta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloncha/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloncha/Documents/GitHub/ISYE6416-Project/data/ejscreen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B52077-3AD3-B146-ADFF-F0FA85DDA297}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDEDE0E-9171-1A4A-BD38-850728B69765}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="460" windowWidth="17000" windowHeight="21620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="460" windowWidth="34600" windowHeight="21620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020_EJSCREEEN_Full_explained" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="270">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -1648,334 +1648,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="70.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="70.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
       <c r="B1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>248</v>
+      </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
       <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
       <c r="B10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B22" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B23" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>11</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>16</v>
-      </c>
-      <c r="B29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>17</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>18</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>19</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>20</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>